<commit_message>
we need this for a more universal issue tracker
</commit_message>
<xml_diff>
--- a/GitToExcel/ReportTemplates/BlankIssues.xlsx
+++ b/GitToExcel/ReportTemplates/BlankIssues.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" iterateCount="1"/>
+  <calcPr calcId="171027" iterate="1" iterateCount="10000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,14 +446,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="33" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" style="4" customWidth="1"/>
     <col min="4" max="4" width="42.33203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="26.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>